<commit_message>
modify scripts to simulate water stage 1 and 2
</commit_message>
<xml_diff>
--- a/Models/Model_2c/ModelData.xlsx
+++ b/Models/Model_2c/ModelData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" tabRatio="714" activeTab="9"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" tabRatio="714" firstSheet="2" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="Dir" sheetId="5" r:id="rId1"/>
@@ -12,11 +12,13 @@
     <sheet name="Rocks" sheetId="1" r:id="rId3"/>
     <sheet name="BC" sheetId="3" r:id="rId4"/>
     <sheet name="NS_Params" sheetId="8" r:id="rId5"/>
-    <sheet name="CO2_S1_BC" sheetId="6" r:id="rId6"/>
-    <sheet name="CO2_S1_Params" sheetId="7" r:id="rId7"/>
-    <sheet name="CO2_S2_BC" sheetId="9" r:id="rId8"/>
-    <sheet name="CO2_S2_Params" sheetId="10" r:id="rId9"/>
-    <sheet name="CO2_hist" sheetId="4" r:id="rId10"/>
+    <sheet name="S1_Params" sheetId="7" r:id="rId6"/>
+    <sheet name="S2_Params" sheetId="10" r:id="rId7"/>
+    <sheet name="hist" sheetId="4" r:id="rId8"/>
+    <sheet name="CO2_S1_BC" sheetId="6" r:id="rId9"/>
+    <sheet name="CO2_S2_BC" sheetId="9" r:id="rId10"/>
+    <sheet name="Water_S1_BC" sheetId="11" r:id="rId11"/>
+    <sheet name="Water_S2_BC" sheetId="13" r:id="rId12"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="97">
   <si>
     <t>ROCK</t>
   </si>
@@ -307,6 +309,18 @@
   </si>
   <si>
     <t>Name</t>
+  </si>
+  <si>
+    <t>inj1</t>
+  </si>
+  <si>
+    <t>prod1</t>
+  </si>
+  <si>
+    <t>prod2</t>
+  </si>
+  <si>
+    <t>prod3</t>
   </si>
 </sst>
 </file>
@@ -696,100 +710,529 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:L11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5703125" customWidth="1"/>
+    <col min="5" max="6" width="8.140625" customWidth="1"/>
+    <col min="7" max="8" width="6.42578125" customWidth="1"/>
+    <col min="9" max="9" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.28515625" customWidth="1"/>
+    <col min="12" max="12" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>92</v>
+        <v>72</v>
       </c>
       <c r="B1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C1" t="s">
         <v>15</v>
       </c>
+      <c r="D1" t="s">
+        <v>70</v>
+      </c>
+      <c r="E1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F1" t="s">
+        <v>68</v>
+      </c>
+      <c r="G1" t="s">
+        <v>69</v>
+      </c>
+      <c r="H1" t="s">
+        <v>26</v>
+      </c>
+      <c r="I1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J1" t="s">
+        <v>28</v>
+      </c>
+      <c r="K1" t="s">
+        <v>66</v>
+      </c>
+      <c r="L1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C2" t="s">
+        <v>64</v>
+      </c>
+      <c r="H2">
+        <v>0.1</v>
+      </c>
+      <c r="I2" s="3">
+        <v>-60</v>
+      </c>
+      <c r="J2" s="1">
+        <v>1000000000000</v>
+      </c>
+      <c r="K2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C3" t="s">
+        <v>64</v>
+      </c>
+      <c r="H3">
+        <v>0.1</v>
+      </c>
+      <c r="I3" s="3">
+        <v>-60</v>
+      </c>
+      <c r="J3" s="1">
+        <v>1000000000000</v>
+      </c>
+      <c r="K3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>73</v>
+      </c>
+      <c r="B4">
+        <v>30</v>
+      </c>
+      <c r="C4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D4" t="s">
+        <v>85</v>
+      </c>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3">
+        <v>750</v>
+      </c>
+      <c r="H4" s="4">
+        <f>-L4*1000000000/(365.25*24*3600)</f>
+        <v>-19.012852688417372</v>
+      </c>
+      <c r="I4" s="3">
+        <v>-60</v>
+      </c>
+      <c r="J4" s="3">
+        <v>1</v>
+      </c>
+      <c r="K4">
+        <v>6</v>
+      </c>
+      <c r="L4" s="4">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>81</v>
+      </c>
+      <c r="B5">
+        <v>31</v>
+      </c>
+      <c r="C5" t="s">
+        <v>64</v>
+      </c>
+      <c r="D5" t="s">
+        <v>84</v>
+      </c>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3">
+        <v>750</v>
+      </c>
+      <c r="H5" s="4">
+        <f>L5*1000000000/(365.25*24*3600)</f>
+        <v>3.1688087814028951</v>
+      </c>
+      <c r="I5" s="3">
+        <v>-60</v>
+      </c>
+      <c r="J5" s="3">
+        <v>1</v>
+      </c>
+      <c r="K5">
+        <v>6</v>
+      </c>
+      <c r="L5" s="4">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>86</v>
+      </c>
+      <c r="B6">
+        <v>32</v>
+      </c>
+      <c r="C6" t="s">
+        <v>64</v>
+      </c>
+      <c r="D6" t="s">
+        <v>87</v>
+      </c>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3">
+        <v>750</v>
+      </c>
+      <c r="H6" s="4">
+        <f>L6*1000000000/(365.25*24*3600)</f>
+        <v>11.724592491190712</v>
+      </c>
+      <c r="I6" s="3">
+        <v>-60</v>
+      </c>
+      <c r="J6" s="3">
+        <v>1</v>
+      </c>
+      <c r="K6">
+        <v>6</v>
+      </c>
+      <c r="L6" s="4">
+        <v>0.37</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>91</v>
+      </c>
+      <c r="B7">
+        <v>33</v>
+      </c>
+      <c r="C7" t="s">
+        <v>64</v>
+      </c>
+      <c r="D7" t="s">
+        <v>89</v>
+      </c>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3">
+        <v>750</v>
+      </c>
+      <c r="H7" s="4">
+        <f>L7*1000000000/(365.25*24*3600)</f>
+        <v>4.1194514158237636</v>
+      </c>
+      <c r="I7" s="3">
+        <v>-60</v>
+      </c>
+      <c r="J7" s="3">
+        <v>1</v>
+      </c>
+      <c r="K7">
+        <v>6</v>
+      </c>
+      <c r="L7" s="4">
+        <v>0.13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J3" sqref="J3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="11.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B1" t="s">
+        <v>65</v>
+      </c>
       <c r="C1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" t="s">
         <v>70</v>
       </c>
+      <c r="E1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F1" t="s">
+        <v>68</v>
+      </c>
+      <c r="G1" t="s">
+        <v>69</v>
+      </c>
+      <c r="H1" t="s">
+        <v>26</v>
+      </c>
+      <c r="I1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J1" t="s">
+        <v>28</v>
+      </c>
+      <c r="K1" t="s">
+        <v>66</v>
+      </c>
+      <c r="L1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>93</v>
+      </c>
+      <c r="B2">
+        <v>30</v>
+      </c>
+      <c r="C2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" t="s">
+        <v>85</v>
+      </c>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3">
+        <v>750</v>
+      </c>
+      <c r="H2" s="4">
+        <f>-L2*1000000000/(365.25*24*3600)</f>
+        <v>-63.376175628057901</v>
+      </c>
+      <c r="I2" s="3">
+        <v>-60</v>
+      </c>
+      <c r="J2" s="3">
+        <v>0</v>
+      </c>
+      <c r="L2" s="3">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C1" t="s">
+        <v>15</v>
+      </c>
       <c r="D1" t="s">
+        <v>70</v>
+      </c>
+      <c r="E1" t="s">
         <v>67</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>68</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H1" t="s">
+        <v>26</v>
+      </c>
+      <c r="I1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J1" t="s">
+        <v>28</v>
+      </c>
+      <c r="K1" t="s">
+        <v>66</v>
+      </c>
+      <c r="L1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>82</v>
-      </c>
-      <c r="B2" t="s">
-        <v>71</v>
+        <v>93</v>
+      </c>
+      <c r="B2">
+        <v>30</v>
       </c>
       <c r="C2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" t="s">
         <v>85</v>
       </c>
-      <c r="D2" s="3"/>
       <c r="E2" s="3"/>
-      <c r="F2" s="3">
+      <c r="F2" s="3"/>
+      <c r="G2" s="3">
         <v>750</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H2" s="4">
+        <f>-L2*1000000000/(365.25*24*3600)</f>
+        <v>-19.012852688417372</v>
+      </c>
+      <c r="I2" s="3">
+        <v>-60</v>
+      </c>
+      <c r="J2" s="3">
+        <v>0</v>
+      </c>
+      <c r="L2" s="4">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>83</v>
-      </c>
-      <c r="B3" t="s">
-        <v>71</v>
+        <v>94</v>
+      </c>
+      <c r="B3">
+        <v>31</v>
       </c>
       <c r="C3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" t="s">
         <v>84</v>
       </c>
-      <c r="D3" s="3"/>
       <c r="E3" s="3"/>
-      <c r="F3" s="3">
+      <c r="F3" s="3"/>
+      <c r="G3" s="3">
         <v>750</v>
       </c>
-      <c r="H3" s="1"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H3" s="4">
+        <f>L3*1000000000/(365.25*24*3600)</f>
+        <v>3.1688087814028951</v>
+      </c>
+      <c r="I3" s="3">
+        <v>-60</v>
+      </c>
+      <c r="J3" s="3">
+        <v>0</v>
+      </c>
+      <c r="L3" s="4">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>88</v>
-      </c>
-      <c r="B4" t="s">
-        <v>71</v>
+        <v>95</v>
+      </c>
+      <c r="B4">
+        <v>32</v>
       </c>
       <c r="C4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" t="s">
         <v>87</v>
       </c>
-      <c r="D4" s="3"/>
       <c r="E4" s="3"/>
-      <c r="F4" s="3">
+      <c r="F4" s="3"/>
+      <c r="G4" s="3">
         <v>750</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H4" s="4">
+        <f>L4*1000000000/(365.25*24*3600)</f>
+        <v>11.724592491190712</v>
+      </c>
+      <c r="I4" s="3">
+        <v>-60</v>
+      </c>
+      <c r="J4" s="3">
+        <v>0</v>
+      </c>
+      <c r="L4" s="4">
+        <v>0.37</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>90</v>
-      </c>
-      <c r="B5" t="s">
-        <v>71</v>
+        <v>96</v>
+      </c>
+      <c r="B5">
+        <v>33</v>
       </c>
       <c r="C5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" t="s">
         <v>89</v>
       </c>
-      <c r="D5" s="3"/>
       <c r="E5" s="3"/>
-      <c r="F5" s="3">
+      <c r="F5" s="3"/>
+      <c r="G5" s="3">
         <v>750</v>
+      </c>
+      <c r="H5" s="4">
+        <f>L5*1000000000/(365.25*24*3600)</f>
+        <v>4.1194514158237636</v>
+      </c>
+      <c r="I5" s="3">
+        <v>-60</v>
+      </c>
+      <c r="J5" s="3">
+        <v>0</v>
+      </c>
+      <c r="L5" s="4">
+        <v>0.13</v>
       </c>
     </row>
   </sheetData>
@@ -1566,7 +2009,7 @@
   <dimension ref="A1:M7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K16" sqref="K16"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1862,10 +2305,260 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>76</v>
+      </c>
+      <c r="B4">
+        <f>365.25*2</f>
+        <v>730.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>77</v>
+      </c>
+      <c r="B5">
+        <f>B4/10</f>
+        <v>73.05</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>78</v>
+      </c>
+      <c r="B6" s="1">
+        <v>1.0000000000000001E-5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>79</v>
+      </c>
+      <c r="B7">
+        <v>3000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L11" sqref="L11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B3">
+        <f>S1_Params!B4</f>
+        <v>730.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>76</v>
+      </c>
+      <c r="B4">
+        <f>365.25*10</f>
+        <v>3652.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>77</v>
+      </c>
+      <c r="B5">
+        <f>B4/10</f>
+        <v>365.25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>78</v>
+      </c>
+      <c r="B6" s="1">
+        <v>1.0000000000000001E-5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>79</v>
+      </c>
+      <c r="B7">
+        <v>5000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E1" t="s">
+        <v>68</v>
+      </c>
+      <c r="F1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C2" t="s">
+        <v>85</v>
+      </c>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>83</v>
+      </c>
+      <c r="B3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C3" t="s">
+        <v>84</v>
+      </c>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3">
+        <v>750</v>
+      </c>
+      <c r="H3" s="1"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>88</v>
+      </c>
+      <c r="B4" t="s">
+        <v>71</v>
+      </c>
+      <c r="C4" t="s">
+        <v>87</v>
+      </c>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>90</v>
+      </c>
+      <c r="B5" t="s">
+        <v>71</v>
+      </c>
+      <c r="C5" t="s">
+        <v>89</v>
+      </c>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3">
+        <v>750</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G8" sqref="A5:G8"/>
+      <selection sqref="A1:L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2027,414 +2720,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>74</v>
-      </c>
-      <c r="B2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>75</v>
-      </c>
-      <c r="B3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>76</v>
-      </c>
-      <c r="B4">
-        <f>365.25*2</f>
-        <v>730.5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>77</v>
-      </c>
-      <c r="B5">
-        <f>B4/10</f>
-        <v>73.05</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>78</v>
-      </c>
-      <c r="B6" s="1">
-        <v>1.0000000000000001E-5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>79</v>
-      </c>
-      <c r="B7">
-        <v>3000</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L11"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G11" sqref="A8:G11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.5703125" customWidth="1"/>
-    <col min="5" max="6" width="8.140625" customWidth="1"/>
-    <col min="7" max="8" width="6.42578125" customWidth="1"/>
-    <col min="9" max="9" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="19.28515625" customWidth="1"/>
-    <col min="12" max="12" width="10.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>72</v>
-      </c>
-      <c r="B1" t="s">
-        <v>65</v>
-      </c>
-      <c r="C1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D1" t="s">
-        <v>70</v>
-      </c>
-      <c r="E1" t="s">
-        <v>67</v>
-      </c>
-      <c r="F1" t="s">
-        <v>68</v>
-      </c>
-      <c r="G1" t="s">
-        <v>69</v>
-      </c>
-      <c r="H1" t="s">
-        <v>26</v>
-      </c>
-      <c r="I1" t="s">
-        <v>27</v>
-      </c>
-      <c r="J1" t="s">
-        <v>28</v>
-      </c>
-      <c r="K1" t="s">
-        <v>66</v>
-      </c>
-      <c r="L1" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>52</v>
-      </c>
-      <c r="C2" t="s">
-        <v>64</v>
-      </c>
-      <c r="H2">
-        <v>0.1</v>
-      </c>
-      <c r="I2" s="3">
-        <v>-60</v>
-      </c>
-      <c r="J2" s="1">
-        <v>1000000000000</v>
-      </c>
-      <c r="K2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>46</v>
-      </c>
-      <c r="C3" t="s">
-        <v>64</v>
-      </c>
-      <c r="H3">
-        <v>0.1</v>
-      </c>
-      <c r="I3" s="3">
-        <v>-60</v>
-      </c>
-      <c r="J3" s="1">
-        <v>1000000000000</v>
-      </c>
-      <c r="K3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>73</v>
-      </c>
-      <c r="B4">
-        <v>30</v>
-      </c>
-      <c r="C4" t="s">
-        <v>64</v>
-      </c>
-      <c r="D4" t="s">
-        <v>85</v>
-      </c>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3">
-        <v>750</v>
-      </c>
-      <c r="H4" s="4">
-        <f>-L4*1000000000/(365.25*24*3600)</f>
-        <v>-19.012852688417372</v>
-      </c>
-      <c r="I4" s="3">
-        <v>-60</v>
-      </c>
-      <c r="J4" s="3">
-        <v>1</v>
-      </c>
-      <c r="K4">
-        <v>6</v>
-      </c>
-      <c r="L4" s="4">
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>81</v>
-      </c>
-      <c r="B5">
-        <v>31</v>
-      </c>
-      <c r="C5" t="s">
-        <v>64</v>
-      </c>
-      <c r="D5" t="s">
-        <v>84</v>
-      </c>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3">
-        <v>750</v>
-      </c>
-      <c r="H5" s="4">
-        <f>L5*1000000000/(365.25*24*3600)</f>
-        <v>3.1688087814028951</v>
-      </c>
-      <c r="I5" s="3">
-        <v>-60</v>
-      </c>
-      <c r="J5" s="3">
-        <v>1</v>
-      </c>
-      <c r="K5">
-        <v>6</v>
-      </c>
-      <c r="L5" s="4">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>86</v>
-      </c>
-      <c r="B6">
-        <v>32</v>
-      </c>
-      <c r="C6" t="s">
-        <v>64</v>
-      </c>
-      <c r="D6" t="s">
-        <v>87</v>
-      </c>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3">
-        <v>750</v>
-      </c>
-      <c r="H6" s="4">
-        <f>L6*1000000000/(365.25*24*3600)</f>
-        <v>11.724592491190712</v>
-      </c>
-      <c r="I6" s="3">
-        <v>-60</v>
-      </c>
-      <c r="J6" s="3">
-        <v>1</v>
-      </c>
-      <c r="K6">
-        <v>6</v>
-      </c>
-      <c r="L6" s="4">
-        <v>0.37</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>91</v>
-      </c>
-      <c r="B7">
-        <v>33</v>
-      </c>
-      <c r="C7" t="s">
-        <v>64</v>
-      </c>
-      <c r="D7" t="s">
-        <v>89</v>
-      </c>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3">
-        <v>750</v>
-      </c>
-      <c r="H7" s="4">
-        <f>L7*1000000000/(365.25*24*3600)</f>
-        <v>4.1194514158237636</v>
-      </c>
-      <c r="I7" s="3">
-        <v>-60</v>
-      </c>
-      <c r="J7" s="3">
-        <v>1</v>
-      </c>
-      <c r="K7">
-        <v>6</v>
-      </c>
-      <c r="L7" s="4">
-        <v>0.13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>74</v>
-      </c>
-      <c r="B2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>75</v>
-      </c>
-      <c r="B3">
-        <f>CO2_S1_Params!B4</f>
-        <v>730.5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>76</v>
-      </c>
-      <c r="B4">
-        <f>365.25*10</f>
-        <v>3652.5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>77</v>
-      </c>
-      <c r="B5">
-        <f>B4/10</f>
-        <v>365.25</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>78</v>
-      </c>
-      <c r="B6" s="1">
-        <v>1.0000000000000001E-5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>79</v>
-      </c>
-      <c r="B7">
-        <v>5000</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>